<commit_message>
Processing excel data and display view added
</commit_message>
<xml_diff>
--- a/Python_For_Machine_Learning/Convert_Excel_To_Pipe_Project/Test.xlsx
+++ b/Python_For_Machine_Learning/Convert_Excel_To_Pipe_Project/Test.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF80235B-DF42-477F-ADB9-4E0796E36DEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -54,12 +55,39 @@
   </si>
   <si>
     <t>FCH</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>08031812695</t>
+  </si>
+  <si>
+    <t>08069784914</t>
+  </si>
+  <si>
+    <t>+2348031812689</t>
+  </si>
+  <si>
+    <t>07029478943</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -89,8 +117,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -184,6 +213,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -219,6 +265,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -394,7 +457,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -451,16 +514,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,8 +539,17 @@
       <c r="E1" t="s">
         <v>8</v>
       </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -493,8 +565,17 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -510,8 +591,14 @@
       <c r="E3" t="s">
         <v>10</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -523,6 +610,12 @@
       </c>
       <c r="E4" t="s">
         <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>